<commit_message>
feat: added new imgs and a new default number of retrains
</commit_message>
<xml_diff>
--- a/forecasts/forecast_2024_06_15.xlsx
+++ b/forecasts/forecast_2024_06_15.xlsx
@@ -520,7 +520,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J2" t="n">
-        <v>0.269001948804676</v>
+        <v>0.2318715247722248</v>
       </c>
     </row>
     <row r="3">
@@ -552,7 +552,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2591697374334894</v>
+        <v>0.2296355541311895</v>
       </c>
     </row>
     <row r="4">
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.227802509170634</v>
+        <v>0.2029956571461736</v>
       </c>
     </row>
     <row r="5">
@@ -616,7 +616,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3557224190550007</v>
+        <v>0.315729021371433</v>
       </c>
     </row>
     <row r="6">
@@ -648,7 +648,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6213655186712967</v>
+        <v>0.588498349146097</v>
       </c>
     </row>
     <row r="7">
@@ -680,7 +680,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4963715415228397</v>
+        <v>0.4580310444726016</v>
       </c>
     </row>
     <row r="8">
@@ -712,7 +712,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3476764871988695</v>
+        <v>0.3075086991600733</v>
       </c>
     </row>
     <row r="9">
@@ -744,7 +744,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2043615705457422</v>
+        <v>0.1844565344153612</v>
       </c>
     </row>
     <row r="10">
@@ -776,7 +776,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J10" t="n">
-        <v>3.564508154411576</v>
+        <v>3.618715793116846</v>
       </c>
     </row>
     <row r="11">
@@ -808,7 +808,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J11" t="n">
-        <v>19.21676567511589</v>
+        <v>19.95230359623808</v>
       </c>
     </row>
     <row r="12">
@@ -840,7 +840,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J12" t="n">
-        <v>25.2758968105308</v>
+        <v>26.04264146543358</v>
       </c>
     </row>
     <row r="13">
@@ -872,7 +872,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J13" t="n">
-        <v>37.13911379702498</v>
+        <v>37.35165333891462</v>
       </c>
     </row>
     <row r="14">
@@ -904,7 +904,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J14" t="n">
-        <v>37.77524097831064</v>
+        <v>37.82649321450703</v>
       </c>
     </row>
     <row r="15">
@@ -936,7 +936,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J15" t="n">
-        <v>37.50882514271408</v>
+        <v>37.71190097676375</v>
       </c>
     </row>
     <row r="16">
@@ -968,7 +968,7 @@
         <v>-1</v>
       </c>
       <c r="J16" t="n">
-        <v>37.52184763012064</v>
+        <v>37.67480693036016</v>
       </c>
     </row>
     <row r="17">
@@ -1000,7 +1000,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J17" t="n">
-        <v>37.45867774894303</v>
+        <v>37.2582695413885</v>
       </c>
     </row>
     <row r="18">
@@ -1032,7 +1032,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J18" t="n">
-        <v>37.96586838315856</v>
+        <v>37.82942910843246</v>
       </c>
     </row>
     <row r="19">
@@ -1064,7 +1064,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J19" t="n">
-        <v>35.69372651515616</v>
+        <v>35.95238334792197</v>
       </c>
     </row>
     <row r="20">
@@ -1096,7 +1096,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J20" t="n">
-        <v>27.1975674409909</v>
+        <v>27.59627743850816</v>
       </c>
     </row>
     <row r="21">
@@ -1128,7 +1128,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J21" t="n">
-        <v>3.950535979557089</v>
+        <v>4.050061987585404</v>
       </c>
     </row>
     <row r="22">
@@ -1160,7 +1160,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5160469653073188</v>
+        <v>0.4794532729108751</v>
       </c>
     </row>
     <row r="23">
@@ -1192,7 +1192,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J23" t="n">
-        <v>0.4138408538137642</v>
+        <v>0.3817444602327352</v>
       </c>
     </row>
     <row r="24">
@@ -1224,7 +1224,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J24" t="n">
-        <v>0.4640517746740925</v>
+        <v>0.4618685549818198</v>
       </c>
     </row>
     <row r="25">
@@ -1256,7 +1256,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J25" t="n">
-        <v>0.2884894136313158</v>
+        <v>0.2753045021439536</v>
       </c>
     </row>
     <row r="26">
@@ -1288,7 +1288,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J26" t="n">
-        <v>0.315159438064483</v>
+        <v>0.3004522680670818</v>
       </c>
     </row>
     <row r="27">
@@ -1320,7 +1320,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J27" t="n">
-        <v>0.2793758185275576</v>
+        <v>0.2508215478899357</v>
       </c>
     </row>
     <row r="28">
@@ -1352,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>0.1304181095230422</v>
+        <v>0.1062099164271934</v>
       </c>
     </row>
     <row r="29">
@@ -1384,7 +1384,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J29" t="n">
-        <v>0.1270035424272848</v>
+        <v>0.1018390717935245</v>
       </c>
     </row>
     <row r="30">
@@ -1416,7 +1416,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J30" t="n">
-        <v>0.08508535127223119</v>
+        <v>0.05901675324555183</v>
       </c>
     </row>
     <row r="31">
@@ -1448,7 +1448,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J31" t="n">
-        <v>0.03464910984134606</v>
+        <v>0.01116247915986296</v>
       </c>
     </row>
     <row r="32">
@@ -1480,7 +1480,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J32" t="n">
-        <v>0.07354854977803543</v>
+        <v>0.06285509121362062</v>
       </c>
     </row>
     <row r="33">
@@ -1512,7 +1512,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J33" t="n">
-        <v>0.2902604573362855</v>
+        <v>0.2758395192031088</v>
       </c>
     </row>
     <row r="34">
@@ -1544,7 +1544,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J34" t="n">
-        <v>3.671797206650338</v>
+        <v>3.655014143589347</v>
       </c>
     </row>
     <row r="35">
@@ -1576,7 +1576,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J35" t="n">
-        <v>11.6395285664394</v>
+        <v>12.05946039681572</v>
       </c>
     </row>
     <row r="36">
@@ -1608,7 +1608,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J36" t="n">
-        <v>24.00082538890067</v>
+        <v>24.96823137666279</v>
       </c>
     </row>
     <row r="37">
@@ -1640,7 +1640,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J37" t="n">
-        <v>30.4263268525039</v>
+        <v>30.7754205926932</v>
       </c>
     </row>
     <row r="38">
@@ -1672,7 +1672,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J38" t="n">
-        <v>28.72908469864885</v>
+        <v>29.13468501863522</v>
       </c>
     </row>
     <row r="39">
@@ -1704,7 +1704,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J39" t="n">
-        <v>34.64353569486946</v>
+        <v>34.49231112304734</v>
       </c>
     </row>
     <row r="40">
@@ -1736,7 +1736,7 @@
         <v>-1</v>
       </c>
       <c r="J40" t="n">
-        <v>40.42696831743577</v>
+        <v>40.69762822969602</v>
       </c>
     </row>
     <row r="41">
@@ -1768,7 +1768,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J41" t="n">
-        <v>39.76088611206223</v>
+        <v>39.95169555091081</v>
       </c>
     </row>
     <row r="42">
@@ -1800,7 +1800,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J42" t="n">
-        <v>37.79636309169148</v>
+        <v>37.28564685957947</v>
       </c>
     </row>
     <row r="43">
@@ -1832,7 +1832,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J43" t="n">
-        <v>31.44305542203132</v>
+        <v>31.64183332729375</v>
       </c>
     </row>
     <row r="44">
@@ -1864,7 +1864,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J44" t="n">
-        <v>19.61515442253404</v>
+        <v>20.32131245441574</v>
       </c>
     </row>
     <row r="45">
@@ -1896,7 +1896,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J45" t="n">
-        <v>2.795175998429959</v>
+        <v>3.091441331583934</v>
       </c>
     </row>
     <row r="46">
@@ -1928,7 +1928,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J46" t="n">
-        <v>0.2507151635091228</v>
+        <v>0.2462197347433333</v>
       </c>
     </row>
     <row r="47">
@@ -1960,7 +1960,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J47" t="n">
-        <v>0.1945670415878206</v>
+        <v>0.1905711464310219</v>
       </c>
     </row>
     <row r="48">
@@ -1992,7 +1992,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J48" t="n">
-        <v>0.2268062272992246</v>
+        <v>0.2311268248327822</v>
       </c>
     </row>
     <row r="49">
@@ -2024,7 +2024,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J49" t="n">
-        <v>0.1572954130654103</v>
+        <v>0.1566482210592247</v>
       </c>
     </row>
     <row r="50">
@@ -2056,7 +2056,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J50" t="n">
-        <v>0.1767209758629639</v>
+        <v>0.1767338579059117</v>
       </c>
     </row>
     <row r="51">
@@ -2088,7 +2088,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J51" t="n">
-        <v>0.1298887610073</v>
+        <v>0.1288905337050665</v>
       </c>
     </row>
     <row r="52">
@@ -2120,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>0.1481793350614303</v>
+        <v>0.147577220811455</v>
       </c>
     </row>
     <row r="53">
@@ -2152,7 +2152,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J53" t="n">
-        <v>0.12344144498668</v>
+        <v>0.1223040198801172</v>
       </c>
     </row>
     <row r="54">
@@ -2184,7 +2184,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J54" t="n">
-        <v>0.2212812620975286</v>
+        <v>0.2222574213032241</v>
       </c>
     </row>
     <row r="55">
@@ -2216,7 +2216,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J55" t="n">
-        <v>0.1295849259004036</v>
+        <v>0.1285813576314633</v>
       </c>
     </row>
     <row r="56">
@@ -2280,7 +2280,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J57" t="n">
-        <v>0.2175238456224222</v>
+        <v>0.2031046112339245</v>
       </c>
     </row>
     <row r="58">
@@ -2312,7 +2312,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J58" t="n">
-        <v>3.454244006830408</v>
+        <v>3.487153476372723</v>
       </c>
     </row>
     <row r="59">
@@ -2344,7 +2344,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J59" t="n">
-        <v>14.57496537567219</v>
+        <v>14.37611957722387</v>
       </c>
     </row>
     <row r="60">
@@ -2376,7 +2376,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J60" t="n">
-        <v>30.78540974642677</v>
+        <v>31.14960977533658</v>
       </c>
     </row>
     <row r="61">
@@ -2408,7 +2408,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J61" t="n">
-        <v>31.50423246180449</v>
+        <v>31.5048894038771</v>
       </c>
     </row>
     <row r="62">
@@ -2440,7 +2440,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J62" t="n">
-        <v>38.17714448331775</v>
+        <v>37.36690161435019</v>
       </c>
     </row>
     <row r="63">
@@ -2472,7 +2472,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J63" t="n">
-        <v>37.88212222162603</v>
+        <v>37.22052461843536</v>
       </c>
     </row>
     <row r="64">
@@ -2504,7 +2504,7 @@
         <v>-1</v>
       </c>
       <c r="J64" t="n">
-        <v>31.097350076352</v>
+        <v>31.52377368770348</v>
       </c>
     </row>
     <row r="65">
@@ -2536,7 +2536,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J65" t="n">
-        <v>37.15796404407265</v>
+        <v>36.28257080786343</v>
       </c>
     </row>
     <row r="66">
@@ -2568,7 +2568,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J66" t="n">
-        <v>28.24956700833583</v>
+        <v>28.91512067005213</v>
       </c>
     </row>
     <row r="67">
@@ -2600,7 +2600,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J67" t="n">
-        <v>31.50024617867308</v>
+        <v>31.55852704582769</v>
       </c>
     </row>
     <row r="68">
@@ -2632,7 +2632,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J68" t="n">
-        <v>19.32728720320536</v>
+        <v>19.85427260974177</v>
       </c>
     </row>
     <row r="69">
@@ -2664,7 +2664,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J69" t="n">
-        <v>2.720900884895087</v>
+        <v>2.917067197191834</v>
       </c>
     </row>
     <row r="70">
@@ -2696,7 +2696,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J70" t="n">
-        <v>0.3445029588735147</v>
+        <v>0.3486096716775575</v>
       </c>
     </row>
     <row r="71">
@@ -2728,7 +2728,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J71" t="n">
-        <v>0.4084445295765827</v>
+        <v>0.4092683427601943</v>
       </c>
     </row>
     <row r="72">
@@ -2760,7 +2760,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J72" t="n">
-        <v>0.3741321150400682</v>
+        <v>0.3817054022792186</v>
       </c>
     </row>
     <row r="73">
@@ -2792,7 +2792,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J73" t="n">
-        <v>0.2404357090729993</v>
+        <v>0.2415321236169505</v>
       </c>
     </row>
     <row r="74">
@@ -2824,7 +2824,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J74" t="n">
-        <v>0.2804775000569052</v>
+        <v>0.2826363225476198</v>
       </c>
     </row>
     <row r="75">
@@ -2856,7 +2856,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J75" t="n">
-        <v>0.3727577124499415</v>
+        <v>0.3769100871702333</v>
       </c>
     </row>
     <row r="76">
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>0.1893265820533603</v>
+        <v>0.1895186715146104</v>
       </c>
     </row>
     <row r="77">
@@ -2920,7 +2920,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J77" t="n">
-        <v>0.1924467778273106</v>
+        <v>0.1927062324370073</v>
       </c>
     </row>
     <row r="78">
@@ -2952,7 +2952,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J78" t="n">
-        <v>0.2044830626918207</v>
+        <v>0.2050146661815595</v>
       </c>
     </row>
     <row r="79">
@@ -2984,7 +2984,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J79" t="n">
-        <v>0.208266017750638</v>
+        <v>0.2088785528638238</v>
       </c>
     </row>
     <row r="80">
@@ -3016,7 +3016,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J80" t="n">
-        <v>0.271298932529643</v>
+        <v>0.2732723507311793</v>
       </c>
     </row>
     <row r="81">
@@ -3048,7 +3048,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J81" t="n">
-        <v>0.3765413714741548</v>
+        <v>0.3649533586004731</v>
       </c>
     </row>
     <row r="82">
@@ -3080,7 +3080,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J82" t="n">
-        <v>3.759541776722342</v>
+        <v>3.793199667066334</v>
       </c>
     </row>
     <row r="83">
@@ -3112,7 +3112,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J83" t="n">
-        <v>11.37893622246844</v>
+        <v>11.56345685771011</v>
       </c>
     </row>
     <row r="84">
@@ -3144,7 +3144,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J84" t="n">
-        <v>29.95618998121034</v>
+        <v>30.34018440592202</v>
       </c>
     </row>
     <row r="85">
@@ -3176,7 +3176,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J85" t="n">
-        <v>37.72571737855226</v>
+        <v>37.13016422371734</v>
       </c>
     </row>
     <row r="86">
@@ -3208,7 +3208,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J86" t="n">
-        <v>39.31903448400009</v>
+        <v>39.57402268040681</v>
       </c>
     </row>
     <row r="87">
@@ -3240,7 +3240,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J87" t="n">
-        <v>39.76552487097433</v>
+        <v>40.30480804649444</v>
       </c>
     </row>
     <row r="88">
@@ -3272,7 +3272,7 @@
         <v>-1</v>
       </c>
       <c r="J88" t="n">
-        <v>39.37131475661943</v>
+        <v>39.5901717826922</v>
       </c>
     </row>
     <row r="89">
@@ -3304,7 +3304,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J89" t="n">
-        <v>37.7754347422953</v>
+        <v>36.94688858988773</v>
       </c>
     </row>
     <row r="90">
@@ -3336,7 +3336,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J90" t="n">
-        <v>30.77550573932999</v>
+        <v>31.61778054437286</v>
       </c>
     </row>
     <row r="91">
@@ -3368,7 +3368,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J91" t="n">
-        <v>26.67012926786248</v>
+        <v>27.79778198187854</v>
       </c>
     </row>
     <row r="92">
@@ -3400,7 +3400,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J92" t="n">
-        <v>19.87202706931481</v>
+        <v>20.62129793812739</v>
       </c>
     </row>
     <row r="93">
@@ -3432,7 +3432,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J93" t="n">
-        <v>6.534399929319194</v>
+        <v>6.710663255064181</v>
       </c>
     </row>
     <row r="94">
@@ -3464,7 +3464,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J94" t="n">
-        <v>1.510516222891547</v>
+        <v>1.375960435319948</v>
       </c>
     </row>
     <row r="95">
@@ -3496,7 +3496,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J95" t="n">
-        <v>0.5430625307687107</v>
+        <v>0.6043215861730348</v>
       </c>
     </row>
     <row r="96">
@@ -3528,7 +3528,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J96" t="n">
-        <v>0.3717610035286273</v>
+        <v>0.4505366395168326</v>
       </c>
     </row>
     <row r="97">
@@ -3560,7 +3560,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J97" t="n">
-        <v>0.0152096050323845</v>
+        <v>0.006736215095962977</v>
       </c>
     </row>
     <row r="98">
@@ -3592,7 +3592,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J98" t="n">
-        <v>0.1807504807774795</v>
+        <v>0.1760490289222561</v>
       </c>
     </row>
     <row r="99">
@@ -3624,7 +3624,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J99" t="n">
-        <v>0.2126906345629333</v>
+        <v>0.2086765599530714</v>
       </c>
     </row>
     <row r="100">
@@ -3656,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="J100" t="n">
-        <v>0.1414646399517747</v>
+        <v>0.1406352550051542</v>
       </c>
     </row>
     <row r="101">
@@ -3688,7 +3688,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J101" t="n">
-        <v>0.2449088826755225</v>
+        <v>0.2463053489638792</v>
       </c>
     </row>
     <row r="102">
@@ -3720,7 +3720,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J102" t="n">
-        <v>0.3364404082078956</v>
+        <v>0.3398129087097093</v>
       </c>
     </row>
     <row r="103">
@@ -3752,7 +3752,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J103" t="n">
-        <v>0.4130179488821593</v>
+        <v>0.41804376147364</v>
       </c>
     </row>
     <row r="104">
@@ -3784,7 +3784,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J104" t="n">
-        <v>0.2896344057746231</v>
+        <v>0.2919963628584772</v>
       </c>
     </row>
     <row r="105">
@@ -3816,7 +3816,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J105" t="n">
-        <v>0.1454002915580734</v>
+        <v>0.1261235960904986</v>
       </c>
     </row>
     <row r="106">
@@ -3848,7 +3848,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J106" t="n">
-        <v>3.474234870403303</v>
+        <v>3.50634273734451</v>
       </c>
     </row>
     <row r="107">
@@ -3880,7 +3880,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J107" t="n">
-        <v>19.92031667899221</v>
+        <v>20.64443667935313</v>
       </c>
     </row>
     <row r="108">
@@ -3912,7 +3912,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J108" t="n">
-        <v>32.41546873229675</v>
+        <v>32.81699808388571</v>
       </c>
     </row>
     <row r="109">
@@ -3944,7 +3944,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J109" t="n">
-        <v>36.56739994865399</v>
+        <v>35.44176349182113</v>
       </c>
     </row>
     <row r="110">
@@ -3976,7 +3976,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J110" t="n">
-        <v>39.57044104172415</v>
+        <v>39.29229987523198</v>
       </c>
     </row>
     <row r="111">
@@ -4008,7 +4008,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J111" t="n">
-        <v>34.96351659682057</v>
+        <v>34.75209969093824</v>
       </c>
     </row>
     <row r="112">
@@ -4040,7 +4040,7 @@
         <v>-1</v>
       </c>
       <c r="J112" t="n">
-        <v>36.16506965232207</v>
+        <v>35.82400863723963</v>
       </c>
     </row>
     <row r="113">
@@ -4072,7 +4072,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J113" t="n">
-        <v>36.10771518500237</v>
+        <v>35.8088102111371</v>
       </c>
     </row>
     <row r="114">
@@ -4104,7 +4104,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J114" t="n">
-        <v>35.0737982721287</v>
+        <v>34.46856179096843</v>
       </c>
     </row>
     <row r="115">
@@ -4136,7 +4136,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J115" t="n">
-        <v>34.34213667876872</v>
+        <v>33.7799760003856</v>
       </c>
     </row>
     <row r="116">
@@ -4168,7 +4168,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J116" t="n">
-        <v>21.0878649072631</v>
+        <v>20.98381748942908</v>
       </c>
     </row>
     <row r="117">
@@ -4200,7 +4200,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J117" t="n">
-        <v>10.19958175445764</v>
+        <v>10.203600135958</v>
       </c>
     </row>
     <row r="118">
@@ -4232,7 +4232,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J118" t="n">
-        <v>2.003059271344583</v>
+        <v>1.700650814396202</v>
       </c>
     </row>
     <row r="119">
@@ -4264,7 +4264,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J119" t="n">
-        <v>1.606607281792409</v>
+        <v>1.553969756029961</v>
       </c>
     </row>
     <row r="120">
@@ -4296,7 +4296,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J120" t="n">
-        <v>1.36591374181743</v>
+        <v>1.740304427874926</v>
       </c>
     </row>
     <row r="121">
@@ -4328,7 +4328,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J121" t="n">
-        <v>0.06480725992530642</v>
+        <v>0.06154019435212751</v>
       </c>
     </row>
     <row r="122">
@@ -4360,7 +4360,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J122" t="n">
-        <v>0.08158984324516824</v>
+        <v>0.0788703283549641</v>
       </c>
     </row>
     <row r="123">
@@ -4392,7 +4392,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J123" t="n">
-        <v>0.133739661579748</v>
+        <v>0.1321467628724231</v>
       </c>
     </row>
     <row r="124">
@@ -4424,7 +4424,7 @@
         <v>1</v>
       </c>
       <c r="J124" t="n">
-        <v>0.2658389315333974</v>
+        <v>0.2670979474929824</v>
       </c>
     </row>
     <row r="125">
@@ -4456,7 +4456,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J125" t="n">
-        <v>0.2618939505340001</v>
+        <v>0.26329489161639</v>
       </c>
     </row>
     <row r="126">
@@ -4488,7 +4488,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J126" t="n">
-        <v>0.1750745564964865</v>
+        <v>0.1738321816785818</v>
       </c>
     </row>
     <row r="127">
@@ -4520,7 +4520,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J127" t="n">
-        <v>0.1458597906858658</v>
+        <v>0.1439866441682938</v>
       </c>
     </row>
     <row r="128">
@@ -4552,7 +4552,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J128" t="n">
-        <v>0.1523660352847046</v>
+        <v>0.1506333826082095</v>
       </c>
     </row>
     <row r="129">
@@ -4584,7 +4584,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J129" t="n">
-        <v>0.1470230427872399</v>
+        <v>0.1287849939421445</v>
       </c>
     </row>
     <row r="130">
@@ -4616,7 +4616,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J130" t="n">
-        <v>3.56634212300395</v>
+        <v>3.614270311946171</v>
       </c>
     </row>
     <row r="131">
@@ -4648,7 +4648,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J131" t="n">
-        <v>20.111904930351</v>
+        <v>20.0724800125493</v>
       </c>
     </row>
     <row r="132">
@@ -4680,7 +4680,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J132" t="n">
-        <v>25.2594036111109</v>
+        <v>25.63644978091755</v>
       </c>
     </row>
     <row r="133">
@@ -4712,7 +4712,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J133" t="n">
-        <v>31.16191261440248</v>
+        <v>30.63700106054456</v>
       </c>
     </row>
     <row r="134">
@@ -4744,7 +4744,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J134" t="n">
-        <v>32.87232400126575</v>
+        <v>32.5913329574354</v>
       </c>
     </row>
     <row r="135">
@@ -4776,7 +4776,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J135" t="n">
-        <v>34.85178980315276</v>
+        <v>34.40574393753864</v>
       </c>
     </row>
     <row r="136">
@@ -4808,7 +4808,7 @@
         <v>-1</v>
       </c>
       <c r="J136" t="n">
-        <v>35.416858426334</v>
+        <v>35.05079052087854</v>
       </c>
     </row>
     <row r="137">
@@ -4840,7 +4840,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J137" t="n">
-        <v>35.42687814308225</v>
+        <v>34.8693717795265</v>
       </c>
     </row>
     <row r="138">
@@ -4872,7 +4872,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J138" t="n">
-        <v>33.88043405715773</v>
+        <v>33.28727194602384</v>
       </c>
     </row>
     <row r="139">
@@ -4904,7 +4904,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J139" t="n">
-        <v>32.06470112750135</v>
+        <v>31.9240419081659</v>
       </c>
     </row>
     <row r="140">
@@ -4936,7 +4936,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J140" t="n">
-        <v>24.91332069001689</v>
+        <v>24.96752512874808</v>
       </c>
     </row>
     <row r="141">
@@ -4968,7 +4968,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J141" t="n">
-        <v>9.147125849189758</v>
+        <v>8.878453322058876</v>
       </c>
     </row>
     <row r="142">
@@ -5000,7 +5000,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J142" t="n">
-        <v>1.308783707682627</v>
+        <v>1.609730880214483</v>
       </c>
     </row>
     <row r="143">
@@ -5032,7 +5032,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J143" t="n">
-        <v>0.9001328744941899</v>
+        <v>1.05891165818381</v>
       </c>
     </row>
     <row r="144">
@@ -5064,7 +5064,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J144" t="n">
-        <v>0.8952359491112124</v>
+        <v>1.037049404886612</v>
       </c>
     </row>
     <row r="145">
@@ -5096,7 +5096,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J145" t="n">
-        <v>0.3470365376585371</v>
+        <v>0.3511163511027831</v>
       </c>
     </row>
     <row r="146">
@@ -5128,7 +5128,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J146" t="n">
-        <v>0.5356178218014586</v>
+        <v>0.5359181363090775</v>
       </c>
     </row>
     <row r="147">
@@ -5160,7 +5160,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J147" t="n">
-        <v>0.6639764289692979</v>
+        <v>0.6748554728708136</v>
       </c>
     </row>
     <row r="148">
@@ -5192,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="J148" t="n">
-        <v>0.534728453356059</v>
+        <v>0.5428709078221202</v>
       </c>
     </row>
     <row r="149">
@@ -5224,7 +5224,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J149" t="n">
-        <v>0.5930176995594223</v>
+        <v>0.5839864391585864</v>
       </c>
     </row>
     <row r="150">
@@ -5256,7 +5256,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J150" t="n">
-        <v>0.407131895816656</v>
+        <v>0.3931991721337897</v>
       </c>
     </row>
     <row r="151">
@@ -5288,7 +5288,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J151" t="n">
-        <v>0.371626141573519</v>
+        <v>0.3569264573130828</v>
       </c>
     </row>
     <row r="152">
@@ -5320,7 +5320,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J152" t="n">
-        <v>10.32204782240358</v>
+        <v>11.52014359597491</v>
       </c>
     </row>
     <row r="153">
@@ -5352,7 +5352,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J153" t="n">
-        <v>13.21471985809016</v>
+        <v>13.63179654454105</v>
       </c>
     </row>
     <row r="154">
@@ -5384,7 +5384,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J154" t="n">
-        <v>11.97788915027637</v>
+        <v>11.17042261425985</v>
       </c>
     </row>
     <row r="155">
@@ -5416,7 +5416,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J155" t="n">
-        <v>24.29647323306317</v>
+        <v>24.16038214021207</v>
       </c>
     </row>
     <row r="156">
@@ -5448,7 +5448,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J156" t="n">
-        <v>29.84575060619596</v>
+        <v>30.10756939884685</v>
       </c>
     </row>
     <row r="157">
@@ -5480,7 +5480,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J157" t="n">
-        <v>33.6389858549498</v>
+        <v>32.58047932780787</v>
       </c>
     </row>
     <row r="158">
@@ -5512,7 +5512,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J158" t="n">
-        <v>33.9755614780851</v>
+        <v>32.9526432641991</v>
       </c>
     </row>
     <row r="159">
@@ -5544,7 +5544,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J159" t="n">
-        <v>33.76573681278068</v>
+        <v>32.76694648080129</v>
       </c>
     </row>
     <row r="160">
@@ -5576,7 +5576,7 @@
         <v>-1</v>
       </c>
       <c r="J160" t="n">
-        <v>33.68281270639664</v>
+        <v>32.76738115788692</v>
       </c>
     </row>
     <row r="161">
@@ -5608,7 +5608,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J161" t="n">
-        <v>33.91793965373659</v>
+        <v>32.98245520713636</v>
       </c>
     </row>
     <row r="162">
@@ -5640,7 +5640,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J162" t="n">
-        <v>34.32351685209819</v>
+        <v>33.75082227964729</v>
       </c>
     </row>
     <row r="163">
@@ -5672,7 +5672,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J163" t="n">
-        <v>34.58717931376052</v>
+        <v>33.81526555327144</v>
       </c>
     </row>
     <row r="164">
@@ -5704,7 +5704,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J164" t="n">
-        <v>22.5081972144283</v>
+        <v>21.99049896056804</v>
       </c>
     </row>
     <row r="165">
@@ -5736,7 +5736,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J165" t="n">
-        <v>12.55363604817607</v>
+        <v>11.72096385411642</v>
       </c>
     </row>
     <row r="166">
@@ -5768,7 +5768,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J166" t="n">
-        <v>11.2808931883827</v>
+        <v>10.53187242348197</v>
       </c>
     </row>
     <row r="167">
@@ -5800,7 +5800,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J167" t="n">
-        <v>11.24644343849254</v>
+        <v>10.51833078042724</v>
       </c>
     </row>
     <row r="168">
@@ -5832,7 +5832,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J168" t="n">
-        <v>15.25762563819875</v>
+        <v>14.93911824154106</v>
       </c>
     </row>
     <row r="169">
@@ -5864,7 +5864,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J169" t="n">
-        <v>5.795804127262441</v>
+        <v>6.598343947816022</v>
       </c>
     </row>
     <row r="170">
@@ -5896,7 +5896,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J170" t="n">
-        <v>5.806817571824341</v>
+        <v>6.641637341350096</v>
       </c>
     </row>
     <row r="171">
@@ -5928,7 +5928,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J171" t="n">
-        <v>5.79728801657022</v>
+        <v>6.556648167691122</v>
       </c>
     </row>
     <row r="172">
@@ -5960,7 +5960,7 @@
         <v>1</v>
       </c>
       <c r="J172" t="n">
-        <v>2.560649950682934</v>
+        <v>2.922905671079679</v>
       </c>
     </row>
     <row r="173">
@@ -5992,7 +5992,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J173" t="n">
-        <v>2.415377857189563</v>
+        <v>2.685697525955243</v>
       </c>
     </row>
     <row r="174">
@@ -6024,7 +6024,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J174" t="n">
-        <v>0.8768210088301769</v>
+        <v>1.043545132732826</v>
       </c>
     </row>
     <row r="175">
@@ -6056,7 +6056,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J175" t="n">
-        <v>0.3178300531665999</v>
+        <v>0.3201315880199795</v>
       </c>
     </row>
     <row r="176">
@@ -6088,7 +6088,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J176" t="n">
-        <v>7.646140224325772</v>
+        <v>8.283882923487043</v>
       </c>
     </row>
     <row r="177">
@@ -6120,7 +6120,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J177" t="n">
-        <v>14.39450601171067</v>
+        <v>15.28127802483989</v>
       </c>
     </row>
     <row r="178">
@@ -6152,7 +6152,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J178" t="n">
-        <v>7.785016404040115</v>
+        <v>7.598505722721985</v>
       </c>
     </row>
     <row r="179">
@@ -6184,7 +6184,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J179" t="n">
-        <v>28.05994158043698</v>
+        <v>28.10062577410911</v>
       </c>
     </row>
     <row r="180">
@@ -6216,7 +6216,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J180" t="n">
-        <v>35.8833416255206</v>
+        <v>35.98613400415577</v>
       </c>
     </row>
     <row r="181">
@@ -6248,7 +6248,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J181" t="n">
-        <v>36.4882500099475</v>
+        <v>36.43731967413488</v>
       </c>
     </row>
     <row r="182">
@@ -6280,7 +6280,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J182" t="n">
-        <v>40.20589250343646</v>
+        <v>40.26138049646323</v>
       </c>
     </row>
     <row r="183">
@@ -6312,7 +6312,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J183" t="n">
-        <v>41.25566234174836</v>
+        <v>41.52553076601586</v>
       </c>
     </row>
     <row r="184">
@@ -6344,7 +6344,7 @@
         <v>-1</v>
       </c>
       <c r="J184" t="n">
-        <v>40.5769505766898</v>
+        <v>40.9182699156338</v>
       </c>
     </row>
     <row r="185">
@@ -6376,7 +6376,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J185" t="n">
-        <v>40.53838287097817</v>
+        <v>40.82230628316507</v>
       </c>
     </row>
     <row r="186">
@@ -6408,7 +6408,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J186" t="n">
-        <v>40.03800466450009</v>
+        <v>40.43296766852744</v>
       </c>
     </row>
     <row r="187">
@@ -6440,7 +6440,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J187" t="n">
-        <v>40.20655862423713</v>
+        <v>40.37588218035592</v>
       </c>
     </row>
     <row r="188">
@@ -6472,7 +6472,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J188" t="n">
-        <v>24.76284469650575</v>
+        <v>24.26381160574591</v>
       </c>
     </row>
     <row r="189">
@@ -6504,7 +6504,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J189" t="n">
-        <v>13.19249392533408</v>
+        <v>12.34972773017513</v>
       </c>
     </row>
     <row r="190">
@@ -6536,7 +6536,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J190" t="n">
-        <v>11.86733215545177</v>
+        <v>11.03508744547038</v>
       </c>
     </row>
     <row r="191">
@@ -6568,7 +6568,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J191" t="n">
-        <v>11.70417787654194</v>
+        <v>10.90972140163064</v>
       </c>
     </row>
     <row r="192">
@@ -6600,7 +6600,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J192" t="n">
-        <v>17.65109456504885</v>
+        <v>17.27030418353498</v>
       </c>
     </row>
     <row r="193">
@@ -6632,7 +6632,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J193" t="n">
-        <v>5.862000577411763</v>
+        <v>6.565091320493725</v>
       </c>
     </row>
     <row r="194">
@@ -6664,7 +6664,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J194" t="n">
-        <v>5.740304913635925</v>
+        <v>6.397129183475689</v>
       </c>
     </row>
     <row r="195">
@@ -6696,7 +6696,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J195" t="n">
-        <v>5.220917761837319</v>
+        <v>5.74756134529847</v>
       </c>
     </row>
     <row r="196">
@@ -6728,7 +6728,7 @@
         <v>1</v>
       </c>
       <c r="J196" t="n">
-        <v>2.080175323266757</v>
+        <v>2.465833867631179</v>
       </c>
     </row>
     <row r="197">
@@ -6760,7 +6760,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J197" t="n">
-        <v>1.895025389947609</v>
+        <v>2.229883765743884</v>
       </c>
     </row>
     <row r="198">
@@ -6792,7 +6792,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J198" t="n">
-        <v>0.6158980884547629</v>
+        <v>0.8487044181623319</v>
       </c>
     </row>
     <row r="199">
@@ -6824,7 +6824,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J199" t="n">
-        <v>0.02645593064230026</v>
+        <v>0.02214262473258277</v>
       </c>
     </row>
     <row r="200">
@@ -6856,7 +6856,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J200" t="n">
-        <v>7.07428430847279</v>
+        <v>7.38493506848084</v>
       </c>
     </row>
     <row r="201">
@@ -6888,7 +6888,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J201" t="n">
-        <v>7.521239323541283</v>
+        <v>7.981729011347279</v>
       </c>
     </row>
     <row r="202">
@@ -6920,7 +6920,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J202" t="n">
-        <v>8.284934690490578</v>
+        <v>8.074614812005018</v>
       </c>
     </row>
     <row r="203">
@@ -6952,7 +6952,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J203" t="n">
-        <v>22.73755406532167</v>
+        <v>23.64653493541162</v>
       </c>
     </row>
     <row r="204">
@@ -6984,7 +6984,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J204" t="n">
-        <v>29.98723321033457</v>
+        <v>29.41353248042616</v>
       </c>
     </row>
     <row r="205">
@@ -7016,7 +7016,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J205" t="n">
-        <v>30.05321254409803</v>
+        <v>29.54214133544959</v>
       </c>
     </row>
     <row r="206">
@@ -7048,7 +7048,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J206" t="n">
-        <v>31.68514409306015</v>
+        <v>31.50458075037544</v>
       </c>
     </row>
     <row r="207">
@@ -7080,7 +7080,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J207" t="n">
-        <v>30.59491421966755</v>
+        <v>30.29567848652841</v>
       </c>
     </row>
     <row r="208">
@@ -7112,7 +7112,7 @@
         <v>-1</v>
       </c>
       <c r="J208" t="n">
-        <v>31.27706433375173</v>
+        <v>30.84572431098714</v>
       </c>
     </row>
     <row r="209">
@@ -7144,7 +7144,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J209" t="n">
-        <v>32.23967490700083</v>
+        <v>31.36035953466624</v>
       </c>
     </row>
     <row r="210">
@@ -7176,7 +7176,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J210" t="n">
-        <v>31.54636159788826</v>
+        <v>31.09355160714052</v>
       </c>
     </row>
     <row r="211">
@@ -7208,7 +7208,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J211" t="n">
-        <v>32.85367338531012</v>
+        <v>32.40137886557444</v>
       </c>
     </row>
     <row r="212">
@@ -7240,7 +7240,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J212" t="n">
-        <v>25.12207395054033</v>
+        <v>25.54727492388686</v>
       </c>
     </row>
     <row r="213">
@@ -7272,7 +7272,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J213" t="n">
-        <v>9.288024167087571</v>
+        <v>9.115601093168319</v>
       </c>
     </row>
     <row r="214">
@@ -7304,7 +7304,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J214" t="n">
-        <v>7.945873775162305</v>
+        <v>7.914043474892862</v>
       </c>
     </row>
     <row r="215">
@@ -7336,7 +7336,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J215" t="n">
-        <v>6.804556774553028</v>
+        <v>6.549360307076551</v>
       </c>
     </row>
     <row r="216">
@@ -7368,7 +7368,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J216" t="n">
-        <v>6.525973581920918</v>
+        <v>6.973564549734427</v>
       </c>
     </row>
     <row r="217">
@@ -7400,7 +7400,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J217" t="n">
-        <v>2.083111613078321</v>
+        <v>2.606293502679467</v>
       </c>
     </row>
     <row r="218">
@@ -7432,7 +7432,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J218" t="n">
-        <v>1.943269108711864</v>
+        <v>2.530994190690369</v>
       </c>
     </row>
     <row r="219">
@@ -7464,7 +7464,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J219" t="n">
-        <v>1.684581667349498</v>
+        <v>2.259845413619828</v>
       </c>
     </row>
     <row r="220">
@@ -7496,7 +7496,7 @@
         <v>1</v>
       </c>
       <c r="J220" t="n">
-        <v>1.256679057401528</v>
+        <v>1.668582461967508</v>
       </c>
     </row>
     <row r="221">
@@ -7528,7 +7528,7 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J221" t="n">
-        <v>1.10059633111364</v>
+        <v>1.283124161041693</v>
       </c>
     </row>
     <row r="222">
@@ -7560,7 +7560,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J222" t="n">
-        <v>0.7893810546717783</v>
+        <v>0.9910794589295536</v>
       </c>
     </row>
     <row r="223">
@@ -7592,7 +7592,7 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J223" t="n">
-        <v>0.147389880294442</v>
+        <v>0.1218864700816773</v>
       </c>
     </row>
     <row r="224">
@@ -7624,7 +7624,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J224" t="n">
-        <v>6.956232612466942</v>
+        <v>7.260157547654828</v>
       </c>
     </row>
     <row r="225">
@@ -7656,7 +7656,7 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J225" t="n">
-        <v>8.401590302144882</v>
+        <v>9.249454032492347</v>
       </c>
     </row>
     <row r="226">
@@ -7688,7 +7688,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J226" t="n">
-        <v>8.23520417978642</v>
+        <v>7.687565651202401</v>
       </c>
     </row>
     <row r="227">
@@ -7720,7 +7720,7 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J227" t="n">
-        <v>26.68967932349369</v>
+        <v>26.44871712235351</v>
       </c>
     </row>
     <row r="228">
@@ -7752,7 +7752,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J228" t="n">
-        <v>32.99266029471202</v>
+        <v>33.01533842702588</v>
       </c>
     </row>
     <row r="229">
@@ -7784,7 +7784,7 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J229" t="n">
-        <v>36.6508499937915</v>
+        <v>36.81958553240867</v>
       </c>
     </row>
     <row r="230">
@@ -7816,7 +7816,7 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J230" t="n">
-        <v>37.17633589376446</v>
+        <v>36.90594757993249</v>
       </c>
     </row>
     <row r="231">
@@ -7848,7 +7848,7 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J231" t="n">
-        <v>36.79506920006443</v>
+        <v>36.54216181591646</v>
       </c>
     </row>
     <row r="232">
@@ -7880,7 +7880,7 @@
         <v>-1</v>
       </c>
       <c r="J232" t="n">
-        <v>37.31116736039604</v>
+        <v>37.32937607460111</v>
       </c>
     </row>
     <row r="233">
@@ -7912,7 +7912,7 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J233" t="n">
-        <v>26.23809641472824</v>
+        <v>28.49226388393222</v>
       </c>
     </row>
     <row r="234">
@@ -7944,7 +7944,7 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J234" t="n">
-        <v>25.74632660738042</v>
+        <v>28.62834635412036</v>
       </c>
     </row>
     <row r="235">
@@ -7976,7 +7976,7 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J235" t="n">
-        <v>26.17629424083137</v>
+        <v>29.33302499021924</v>
       </c>
     </row>
     <row r="236">
@@ -8008,7 +8008,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J236" t="n">
-        <v>26.30960600709782</v>
+        <v>26.02168973119664</v>
       </c>
     </row>
     <row r="237">
@@ -8040,7 +8040,7 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J237" t="n">
-        <v>12.93026505922232</v>
+        <v>12.23837614895604</v>
       </c>
     </row>
     <row r="238">
@@ -8072,7 +8072,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J238" t="n">
-        <v>7.810598516677604</v>
+        <v>7.700293269590694</v>
       </c>
     </row>
     <row r="239">
@@ -8104,7 +8104,7 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J239" t="n">
-        <v>7.312551665334762</v>
+        <v>7.283542118443312</v>
       </c>
     </row>
     <row r="240">
@@ -8136,7 +8136,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J240" t="n">
-        <v>7.886441669399597</v>
+        <v>8.436624725004442</v>
       </c>
     </row>
     <row r="241">
@@ -8168,7 +8168,7 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J241" t="n">
-        <v>0.5413706398264945</v>
+        <v>0.5731499887779635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: changed model config and added bias removal for forecasts
</commit_message>
<xml_diff>
--- a/forecasts/forecast_2024_06_15.xlsx
+++ b/forecasts/forecast_2024_06_15.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J241"/>
+  <dimension ref="A1:L241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,16 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>sin(month)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>cos(month)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>generation</t>
         </is>
       </c>
@@ -520,7 +530,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2318715247722248</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -552,7 +568,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2296355541311895</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -584,7 +606,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2029956571461736</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -616,7 +644,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J5" t="n">
-        <v>0.315729021371433</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -648,7 +682,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J6" t="n">
-        <v>0.588498349146097</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -680,7 +720,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4580310444726016</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -712,7 +758,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3075086991600733</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -744,7 +796,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1844565344153612</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -776,7 +834,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J10" t="n">
-        <v>3.618715793116846</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2.470892583227245</v>
       </c>
     </row>
     <row r="11">
@@ -808,7 +872,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J11" t="n">
-        <v>19.95230359623808</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>25.42258975247744</v>
       </c>
     </row>
     <row r="12">
@@ -840,7 +910,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J12" t="n">
-        <v>26.04264146543358</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>33.37048717288993</v>
       </c>
     </row>
     <row r="13">
@@ -872,7 +948,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J13" t="n">
-        <v>37.35165333891462</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L13" t="n">
+        <v>43.88909040533794</v>
       </c>
     </row>
     <row r="14">
@@ -904,7 +986,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J14" t="n">
-        <v>37.82649321450703</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L14" t="n">
+        <v>44.59378108667335</v>
       </c>
     </row>
     <row r="15">
@@ -936,7 +1024,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J15" t="n">
-        <v>37.71190097676375</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>45.08028801622658</v>
       </c>
     </row>
     <row r="16">
@@ -968,7 +1062,13 @@
         <v>-1</v>
       </c>
       <c r="J16" t="n">
-        <v>37.67480693036016</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>44.63588814742042</v>
       </c>
     </row>
     <row r="17">
@@ -1000,7 +1100,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J17" t="n">
-        <v>37.2582695413885</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L17" t="n">
+        <v>46.29621655143952</v>
       </c>
     </row>
     <row r="18">
@@ -1032,7 +1138,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J18" t="n">
-        <v>37.82942910843246</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>42.46227831776728</v>
       </c>
     </row>
     <row r="19">
@@ -1064,7 +1176,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J19" t="n">
-        <v>35.95238334792197</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L19" t="n">
+        <v>41.68209796399416</v>
       </c>
     </row>
     <row r="20">
@@ -1096,7 +1214,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J20" t="n">
-        <v>27.59627743850816</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L20" t="n">
+        <v>17.57333628029826</v>
       </c>
     </row>
     <row r="21">
@@ -1128,7 +1252,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J21" t="n">
-        <v>4.050061987585404</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.2700066969582813</v>
       </c>
     </row>
     <row r="22">
@@ -1160,7 +1290,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J22" t="n">
-        <v>0.4794532729108751</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1192,7 +1328,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J23" t="n">
-        <v>0.3817444602327352</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1224,7 +1366,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J24" t="n">
-        <v>0.4618685549818198</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1256,7 +1404,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J25" t="n">
-        <v>0.2753045021439536</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1288,7 +1442,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J26" t="n">
-        <v>0.3004522680670818</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1320,7 +1480,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J27" t="n">
-        <v>0.2508215478899357</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1352,7 +1518,13 @@
         <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>0.1062099164271934</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1384,7 +1556,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J29" t="n">
-        <v>0.1018390717935245</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1416,7 +1594,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J30" t="n">
-        <v>0.05901675324555183</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1448,7 +1632,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J31" t="n">
-        <v>0.01116247915986296</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1480,7 +1670,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J32" t="n">
-        <v>0.06285509121362062</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1512,7 +1708,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J33" t="n">
-        <v>0.2758395192031088</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K33" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1544,7 +1746,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J34" t="n">
-        <v>3.655014143589347</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L34" t="n">
+        <v>2.522743375046202</v>
       </c>
     </row>
     <row r="35">
@@ -1576,7 +1784,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J35" t="n">
-        <v>12.05946039681572</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K35" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>17.26155461934031</v>
       </c>
     </row>
     <row r="36">
@@ -1608,7 +1822,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J36" t="n">
-        <v>24.96823137666279</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K36" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L36" t="n">
+        <v>31.36308109078835</v>
       </c>
     </row>
     <row r="37">
@@ -1640,7 +1860,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J37" t="n">
-        <v>30.7754205926932</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L37" t="n">
+        <v>33.91166916305204</v>
       </c>
     </row>
     <row r="38">
@@ -1672,7 +1898,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J38" t="n">
-        <v>29.13468501863522</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L38" t="n">
+        <v>34.70928806371096</v>
       </c>
     </row>
     <row r="39">
@@ -1704,7 +1936,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J39" t="n">
-        <v>34.49231112304734</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K39" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L39" t="n">
+        <v>40.26414500401375</v>
       </c>
     </row>
     <row r="40">
@@ -1736,7 +1974,13 @@
         <v>-1</v>
       </c>
       <c r="J40" t="n">
-        <v>40.69762822969602</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K40" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L40" t="n">
+        <v>42.06169194870285</v>
       </c>
     </row>
     <row r="41">
@@ -1768,7 +2012,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J41" t="n">
-        <v>39.95169555091081</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K41" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L41" t="n">
+        <v>44.61232953192369</v>
       </c>
     </row>
     <row r="42">
@@ -1800,7 +2050,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J42" t="n">
-        <v>37.28564685957947</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K42" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L42" t="n">
+        <v>44.29164498003252</v>
       </c>
     </row>
     <row r="43">
@@ -1832,7 +2088,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J43" t="n">
-        <v>31.64183332729375</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K43" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L43" t="n">
+        <v>37.56658551264714</v>
       </c>
     </row>
     <row r="44">
@@ -1864,7 +2126,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J44" t="n">
-        <v>20.32131245441574</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K44" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L44" t="n">
+        <v>16.29576854324043</v>
       </c>
     </row>
     <row r="45">
@@ -1896,7 +2164,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J45" t="n">
-        <v>3.091441331583934</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K45" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0.2266278454728039</v>
       </c>
     </row>
     <row r="46">
@@ -1928,7 +2202,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J46" t="n">
-        <v>0.2462197347433333</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K46" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1960,7 +2240,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J47" t="n">
-        <v>0.1905711464310219</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K47" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1992,7 +2278,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J48" t="n">
-        <v>0.2311268248327822</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K48" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2024,7 +2316,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J49" t="n">
-        <v>0.1566482210592247</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K49" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2056,7 +2354,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J50" t="n">
-        <v>0.1767338579059117</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2088,7 +2392,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J51" t="n">
-        <v>0.1288905337050665</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K51" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2120,7 +2430,13 @@
         <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>0.147577220811455</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K52" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2152,7 +2468,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J53" t="n">
-        <v>0.1223040198801172</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K53" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2184,7 +2506,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J54" t="n">
-        <v>0.2222574213032241</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K54" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2216,7 +2544,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J55" t="n">
-        <v>0.1285813576314633</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K55" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2248,6 +2582,12 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J56" t="n">
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K56" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2280,7 +2620,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J57" t="n">
-        <v>0.2031046112339245</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K57" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2312,7 +2658,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J58" t="n">
-        <v>3.487153476372723</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K58" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L58" t="n">
+        <v>2.175728787762586</v>
       </c>
     </row>
     <row r="59">
@@ -2344,7 +2696,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J59" t="n">
-        <v>14.37611957722387</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K59" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L59" t="n">
+        <v>19.11510222135874</v>
       </c>
     </row>
     <row r="60">
@@ -2376,7 +2734,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J60" t="n">
-        <v>31.14960977533658</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K60" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L60" t="n">
+        <v>34.45781518338279</v>
       </c>
     </row>
     <row r="61">
@@ -2408,7 +2772,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J61" t="n">
-        <v>31.5048894038771</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K61" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L61" t="n">
+        <v>35.58089269356103</v>
       </c>
     </row>
     <row r="62">
@@ -2440,7 +2810,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J62" t="n">
-        <v>37.36690161435019</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K62" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L62" t="n">
+        <v>42.71054156018931</v>
       </c>
     </row>
     <row r="63">
@@ -2472,7 +2848,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J63" t="n">
-        <v>37.22052461843536</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K63" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L63" t="n">
+        <v>42.16586480828276</v>
       </c>
     </row>
     <row r="64">
@@ -2504,7 +2886,13 @@
         <v>-1</v>
       </c>
       <c r="J64" t="n">
-        <v>31.52377368770348</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K64" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L64" t="n">
+        <v>37.80049024482152</v>
       </c>
     </row>
     <row r="65">
@@ -2536,7 +2924,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J65" t="n">
-        <v>36.28257080786343</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K65" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L65" t="n">
+        <v>45.74688274145615</v>
       </c>
     </row>
     <row r="66">
@@ -2568,7 +2962,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J66" t="n">
-        <v>28.91512067005213</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K66" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L66" t="n">
+        <v>38.56886300878801</v>
       </c>
     </row>
     <row r="67">
@@ -2600,7 +3000,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J67" t="n">
-        <v>31.55852704582769</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K67" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L67" t="n">
+        <v>36.51134286400479</v>
       </c>
     </row>
     <row r="68">
@@ -2632,7 +3038,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J68" t="n">
-        <v>19.85427260974177</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K68" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L68" t="n">
+        <v>16.38503987655877</v>
       </c>
     </row>
     <row r="69">
@@ -2664,7 +3076,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J69" t="n">
-        <v>2.917067197191834</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K69" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0.2187280041309632</v>
       </c>
     </row>
     <row r="70">
@@ -2696,7 +3114,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J70" t="n">
-        <v>0.3486096716775575</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K70" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2728,7 +3152,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J71" t="n">
-        <v>0.4092683427601943</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K71" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2760,7 +3190,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J72" t="n">
-        <v>0.3817054022792186</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K72" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2792,7 +3228,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J73" t="n">
-        <v>0.2415321236169505</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K73" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2824,7 +3266,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J74" t="n">
-        <v>0.2826363225476198</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K74" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2856,7 +3304,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J75" t="n">
-        <v>0.3769100871702333</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K75" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2888,7 +3342,13 @@
         <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>0.1895186715146104</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K76" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2920,7 +3380,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J77" t="n">
-        <v>0.1927062324370073</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K77" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2952,7 +3418,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J78" t="n">
-        <v>0.2050146661815595</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K78" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2984,7 +3456,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J79" t="n">
-        <v>0.2088785528638238</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K79" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -3016,7 +3494,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J80" t="n">
-        <v>0.2732723507311793</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K80" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3048,7 +3532,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J81" t="n">
-        <v>0.3649533586004731</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K81" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -3080,7 +3570,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J82" t="n">
-        <v>3.793199667066334</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K82" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L82" t="n">
+        <v>2.276097305487372</v>
       </c>
     </row>
     <row r="83">
@@ -3112,7 +3608,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J83" t="n">
-        <v>11.56345685771011</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K83" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L83" t="n">
+        <v>16.46636307603976</v>
       </c>
     </row>
     <row r="84">
@@ -3144,7 +3646,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J84" t="n">
-        <v>30.34018440592202</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K84" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L84" t="n">
+        <v>34.86067134550577</v>
       </c>
     </row>
     <row r="85">
@@ -3176,7 +3684,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J85" t="n">
-        <v>37.13016422371734</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K85" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L85" t="n">
+        <v>43.74921167467043</v>
       </c>
     </row>
     <row r="86">
@@ -3208,7 +3722,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J86" t="n">
-        <v>39.57402268040681</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K86" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L86" t="n">
+        <v>43.35259055580709</v>
       </c>
     </row>
     <row r="87">
@@ -3240,7 +3760,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J87" t="n">
-        <v>40.30480804649444</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K87" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L87" t="n">
+        <v>42.58257990445016</v>
       </c>
     </row>
     <row r="88">
@@ -3272,7 +3798,13 @@
         <v>-1</v>
       </c>
       <c r="J88" t="n">
-        <v>39.5901717826922</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K88" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L88" t="n">
+        <v>43.41012490474471</v>
       </c>
     </row>
     <row r="89">
@@ -3304,7 +3836,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J89" t="n">
-        <v>36.94688858988773</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K89" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L89" t="n">
+        <v>45.84939398532318</v>
       </c>
     </row>
     <row r="90">
@@ -3336,7 +3874,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J90" t="n">
-        <v>31.61778054437286</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K90" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L90" t="n">
+        <v>39.17733275093201</v>
       </c>
     </row>
     <row r="91">
@@ -3368,7 +3912,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J91" t="n">
-        <v>27.79778198187854</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K91" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L91" t="n">
+        <v>37.16420510178793</v>
       </c>
     </row>
     <row r="92">
@@ -3400,7 +3950,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J92" t="n">
-        <v>20.62129793812739</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K92" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L92" t="n">
+        <v>18.07963432540278</v>
       </c>
     </row>
     <row r="93">
@@ -3432,7 +3988,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J93" t="n">
-        <v>6.710663255064181</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K93" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L93" t="n">
+        <v>0.4137214861356666</v>
       </c>
     </row>
     <row r="94">
@@ -3464,7 +4026,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J94" t="n">
-        <v>1.375960435319948</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K94" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L94" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -3496,7 +4064,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J95" t="n">
-        <v>0.6043215861730348</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K95" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L95" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3528,7 +4102,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J96" t="n">
-        <v>0.4505366395168326</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K96" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -3560,7 +4140,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J97" t="n">
-        <v>0.006736215095962977</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K97" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L97" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -3592,7 +4178,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J98" t="n">
-        <v>0.1760490289222561</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K98" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L98" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -3624,7 +4216,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J99" t="n">
-        <v>0.2086765599530714</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K99" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L99" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3656,7 +4254,13 @@
         <v>1</v>
       </c>
       <c r="J100" t="n">
-        <v>0.1406352550051542</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L100" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -3688,7 +4292,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J101" t="n">
-        <v>0.2463053489638792</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K101" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L101" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -3720,7 +4330,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J102" t="n">
-        <v>0.3398129087097093</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K102" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L102" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -3752,7 +4368,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J103" t="n">
-        <v>0.41804376147364</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K103" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L103" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -3784,7 +4406,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J104" t="n">
-        <v>0.2919963628584772</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K104" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L104" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -3816,7 +4444,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J105" t="n">
-        <v>0.1261235960904986</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K105" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L105" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -3848,7 +4482,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J106" t="n">
-        <v>3.50634273734451</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K106" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L106" t="n">
+        <v>2.070544206950493</v>
       </c>
     </row>
     <row r="107">
@@ -3880,7 +4520,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J107" t="n">
-        <v>20.64443667935313</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K107" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L107" t="n">
+        <v>27.72679422122621</v>
       </c>
     </row>
     <row r="108">
@@ -3912,7 +4558,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J108" t="n">
-        <v>32.81699808388571</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K108" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L108" t="n">
+        <v>34.2112390771422</v>
       </c>
     </row>
     <row r="109">
@@ -3944,7 +4596,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J109" t="n">
-        <v>35.44176349182113</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K109" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L109" t="n">
+        <v>39.77938755294564</v>
       </c>
     </row>
     <row r="110">
@@ -3976,7 +4634,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J110" t="n">
-        <v>39.29229987523198</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K110" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L110" t="n">
+        <v>40.28870825544946</v>
       </c>
     </row>
     <row r="111">
@@ -4008,7 +4672,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J111" t="n">
-        <v>34.75209969093824</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K111" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L111" t="n">
+        <v>40.02167571960383</v>
       </c>
     </row>
     <row r="112">
@@ -4040,7 +4710,13 @@
         <v>-1</v>
       </c>
       <c r="J112" t="n">
-        <v>35.82400863723963</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K112" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L112" t="n">
+        <v>41.56892482998342</v>
       </c>
     </row>
     <row r="113">
@@ -4072,7 +4748,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J113" t="n">
-        <v>35.8088102111371</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K113" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L113" t="n">
+        <v>43.60393936487225</v>
       </c>
     </row>
     <row r="114">
@@ -4104,7 +4786,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J114" t="n">
-        <v>34.46856179096843</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K114" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L114" t="n">
+        <v>43.36043150689942</v>
       </c>
     </row>
     <row r="115">
@@ -4136,7 +4824,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J115" t="n">
-        <v>33.7799760003856</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K115" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L115" t="n">
+        <v>41.74315159530468</v>
       </c>
     </row>
     <row r="116">
@@ -4168,7 +4862,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J116" t="n">
-        <v>20.98381748942908</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K116" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L116" t="n">
+        <v>16.43378284487721</v>
       </c>
     </row>
     <row r="117">
@@ -4200,7 +4900,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J117" t="n">
-        <v>10.203600135958</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K117" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L117" t="n">
+        <v>0.7374401224656868</v>
       </c>
     </row>
     <row r="118">
@@ -4232,7 +4938,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J118" t="n">
-        <v>1.700650814396202</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K118" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L118" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -4264,7 +4976,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J119" t="n">
-        <v>1.553969756029961</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K119" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L119" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -4296,7 +5014,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J120" t="n">
-        <v>1.740304427874926</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K120" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L120" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -4328,7 +5052,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J121" t="n">
-        <v>0.06154019435212751</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K121" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L121" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -4360,7 +5090,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J122" t="n">
-        <v>0.0788703283549641</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K122" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L122" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -4392,7 +5128,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J123" t="n">
-        <v>0.1321467628724231</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K123" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L123" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -4424,7 +5166,13 @@
         <v>1</v>
       </c>
       <c r="J124" t="n">
-        <v>0.2670979474929824</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K124" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L124" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -4456,7 +5204,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J125" t="n">
-        <v>0.26329489161639</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K125" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L125" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -4488,7 +5242,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J126" t="n">
-        <v>0.1738321816785818</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K126" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L126" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -4520,7 +5280,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J127" t="n">
-        <v>0.1439866441682938</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K127" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L127" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -4552,7 +5318,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J128" t="n">
-        <v>0.1506333826082095</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K128" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L128" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -4584,7 +5356,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J129" t="n">
-        <v>0.1287849939421445</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K129" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L129" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -4616,7 +5394,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J130" t="n">
-        <v>3.614270311946171</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K130" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L130" t="n">
+        <v>2.189983188970579</v>
       </c>
     </row>
     <row r="131">
@@ -4648,7 +5432,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J131" t="n">
-        <v>20.0724800125493</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K131" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L131" t="n">
+        <v>28.84132296146034</v>
       </c>
     </row>
     <row r="132">
@@ -4680,7 +5470,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J132" t="n">
-        <v>25.63644978091755</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K132" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L132" t="n">
+        <v>33.98354576177094</v>
       </c>
     </row>
     <row r="133">
@@ -4712,7 +5508,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J133" t="n">
-        <v>30.63700106054456</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K133" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L133" t="n">
+        <v>39.70272870092158</v>
       </c>
     </row>
     <row r="134">
@@ -4744,7 +5546,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J134" t="n">
-        <v>32.5913329574354</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K134" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L134" t="n">
+        <v>40.76504208629508</v>
       </c>
     </row>
     <row r="135">
@@ -4776,7 +5584,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J135" t="n">
-        <v>34.40574393753864</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K135" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L135" t="n">
+        <v>41.13091591776765</v>
       </c>
     </row>
     <row r="136">
@@ -4808,7 +5622,13 @@
         <v>-1</v>
       </c>
       <c r="J136" t="n">
-        <v>35.05079052087854</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K136" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L136" t="n">
+        <v>42.26897419810323</v>
       </c>
     </row>
     <row r="137">
@@ -4840,7 +5660,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J137" t="n">
-        <v>34.8693717795265</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K137" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L137" t="n">
+        <v>44.27287694573207</v>
       </c>
     </row>
     <row r="138">
@@ -4872,7 +5698,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J138" t="n">
-        <v>33.28727194602384</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K138" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L138" t="n">
+        <v>43.38018161658726</v>
       </c>
     </row>
     <row r="139">
@@ -4904,7 +5736,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J139" t="n">
-        <v>31.9240419081659</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K139" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L139" t="n">
+        <v>42.0217512638611</v>
       </c>
     </row>
     <row r="140">
@@ -4936,7 +5774,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J140" t="n">
-        <v>24.96752512874808</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K140" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L140" t="n">
+        <v>15.99360851002872</v>
       </c>
     </row>
     <row r="141">
@@ -4968,7 +5812,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J141" t="n">
-        <v>8.878453322058876</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K141" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L141" t="n">
+        <v>0.5714959327213984</v>
       </c>
     </row>
     <row r="142">
@@ -5000,7 +5850,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J142" t="n">
-        <v>1.609730880214483</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K142" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L142" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -5032,7 +5888,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J143" t="n">
-        <v>1.05891165818381</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K143" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L143" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -5064,7 +5926,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J144" t="n">
-        <v>1.037049404886612</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K144" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L144" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -5096,7 +5964,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J145" t="n">
-        <v>0.3511163511027831</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K145" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L145" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -5128,7 +6002,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J146" t="n">
-        <v>0.5359181363090775</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K146" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L146" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -5160,7 +6040,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J147" t="n">
-        <v>0.6748554728708136</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K147" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L147" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -5192,7 +6078,13 @@
         <v>1</v>
       </c>
       <c r="J148" t="n">
-        <v>0.5428709078221202</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K148" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L148" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -5224,7 +6116,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J149" t="n">
-        <v>0.5839864391585864</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K149" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L149" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -5256,7 +6154,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J150" t="n">
-        <v>0.3931991721337897</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K150" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L150" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -5288,7 +6192,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J151" t="n">
-        <v>0.3569264573130828</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K151" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L151" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -5320,7 +6230,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J152" t="n">
-        <v>11.52014359597491</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K152" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L152" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -5352,7 +6268,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J153" t="n">
-        <v>13.63179654454105</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K153" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L153" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -5384,7 +6306,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J154" t="n">
-        <v>11.17042261425985</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K154" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L154" t="n">
+        <v>7.793190396760623</v>
       </c>
     </row>
     <row r="155">
@@ -5416,7 +6344,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J155" t="n">
-        <v>24.16038214021207</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K155" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L155" t="n">
+        <v>29.49949004991371</v>
       </c>
     </row>
     <row r="156">
@@ -5448,7 +6382,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J156" t="n">
-        <v>30.10756939884685</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K156" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L156" t="n">
+        <v>36.09503785175491</v>
       </c>
     </row>
     <row r="157">
@@ -5480,7 +6420,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J157" t="n">
-        <v>32.58047932780787</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K157" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L157" t="n">
+        <v>36.97992391656099</v>
       </c>
     </row>
     <row r="158">
@@ -5512,7 +6458,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J158" t="n">
-        <v>32.9526432641991</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K158" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L158" t="n">
+        <v>39.91284379741397</v>
       </c>
     </row>
     <row r="159">
@@ -5544,7 +6496,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J159" t="n">
-        <v>32.76694648080129</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K159" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L159" t="n">
+        <v>39.87351396805871</v>
       </c>
     </row>
     <row r="160">
@@ -5576,7 +6534,13 @@
         <v>-1</v>
       </c>
       <c r="J160" t="n">
-        <v>32.76738115788692</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K160" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L160" t="n">
+        <v>40.9203593655463</v>
       </c>
     </row>
     <row r="161">
@@ -5608,7 +6572,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J161" t="n">
-        <v>32.98245520713636</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K161" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L161" t="n">
+        <v>43.57199031874277</v>
       </c>
     </row>
     <row r="162">
@@ -5640,7 +6610,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J162" t="n">
-        <v>33.75082227964729</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K162" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L162" t="n">
+        <v>43.09689423878689</v>
       </c>
     </row>
     <row r="163">
@@ -5672,7 +6648,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J163" t="n">
-        <v>33.81526555327144</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K163" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L163" t="n">
+        <v>41.43306007203031</v>
       </c>
     </row>
     <row r="164">
@@ -5704,7 +6686,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J164" t="n">
-        <v>21.99049896056804</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K164" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L164" t="n">
+        <v>16.12862769332268</v>
       </c>
     </row>
     <row r="165">
@@ -5736,7 +6724,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J165" t="n">
-        <v>11.72096385411642</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K165" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L165" t="n">
+        <v>0.9003197326441867</v>
       </c>
     </row>
     <row r="166">
@@ -5768,7 +6762,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J166" t="n">
-        <v>10.53187242348197</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K166" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L166" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -5800,7 +6800,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J167" t="n">
-        <v>10.51833078042724</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K167" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L167" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -5832,7 +6838,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J168" t="n">
-        <v>14.93911824154106</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K168" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L168" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -5864,7 +6876,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J169" t="n">
-        <v>6.598343947816022</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K169" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L169" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -5896,7 +6914,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J170" t="n">
-        <v>6.641637341350096</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K170" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L170" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -5928,7 +6952,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J171" t="n">
-        <v>6.556648167691122</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K171" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L171" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -5960,7 +6990,13 @@
         <v>1</v>
       </c>
       <c r="J172" t="n">
-        <v>2.922905671079679</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K172" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L172" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -5992,7 +7028,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J173" t="n">
-        <v>2.685697525955243</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K173" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L173" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -6024,7 +7066,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J174" t="n">
-        <v>1.043545132732826</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K174" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L174" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -6056,7 +7104,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J175" t="n">
-        <v>0.3201315880199795</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K175" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L175" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="176">
@@ -6088,7 +7142,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J176" t="n">
-        <v>8.283882923487043</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K176" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L176" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -6120,7 +7180,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J177" t="n">
-        <v>15.28127802483989</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K177" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L177" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -6152,7 +7218,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J178" t="n">
-        <v>7.598505722721985</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K178" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L178" t="n">
+        <v>8.215723868290775</v>
       </c>
     </row>
     <row r="179">
@@ -6184,7 +7256,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J179" t="n">
-        <v>28.10062577410911</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K179" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L179" t="n">
+        <v>32.73350921898456</v>
       </c>
     </row>
     <row r="180">
@@ -6216,7 +7294,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J180" t="n">
-        <v>35.98613400415577</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K180" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L180" t="n">
+        <v>43.12113474215423</v>
       </c>
     </row>
     <row r="181">
@@ -6248,7 +7332,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J181" t="n">
-        <v>36.43731967413488</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K181" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L181" t="n">
+        <v>42.40292321748865</v>
       </c>
     </row>
     <row r="182">
@@ -6280,7 +7370,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J182" t="n">
-        <v>40.26138049646323</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K182" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L182" t="n">
+        <v>41.48758147134932</v>
       </c>
     </row>
     <row r="183">
@@ -6312,7 +7408,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J183" t="n">
-        <v>41.52553076601586</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K183" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L183" t="n">
+        <v>41.17571341025497</v>
       </c>
     </row>
     <row r="184">
@@ -6344,7 +7446,13 @@
         <v>-1</v>
       </c>
       <c r="J184" t="n">
-        <v>40.9182699156338</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K184" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L184" t="n">
+        <v>42.99476730175563</v>
       </c>
     </row>
     <row r="185">
@@ -6376,7 +7484,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J185" t="n">
-        <v>40.82230628316507</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K185" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L185" t="n">
+        <v>43.51474283991588</v>
       </c>
     </row>
     <row r="186">
@@ -6408,7 +7522,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J186" t="n">
-        <v>40.43296766852744</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K186" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L186" t="n">
+        <v>39.76778497859912</v>
       </c>
     </row>
     <row r="187">
@@ -6440,7 +7560,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J187" t="n">
-        <v>40.37588218035592</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K187" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L187" t="n">
+        <v>38.40868898879853</v>
       </c>
     </row>
     <row r="188">
@@ -6472,7 +7598,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J188" t="n">
-        <v>24.26381160574591</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K188" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L188" t="n">
+        <v>20.35227059182423</v>
       </c>
     </row>
     <row r="189">
@@ -6504,7 +7636,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J189" t="n">
-        <v>12.34972773017513</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K189" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L189" t="n">
+        <v>1.031250169063561</v>
       </c>
     </row>
     <row r="190">
@@ -6536,7 +7674,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J190" t="n">
-        <v>11.03508744547038</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K190" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L190" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="191">
@@ -6568,7 +7712,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J191" t="n">
-        <v>10.90972140163064</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K191" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L191" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -6600,7 +7750,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J192" t="n">
-        <v>17.27030418353498</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K192" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L192" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -6632,7 +7788,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J193" t="n">
-        <v>6.565091320493725</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K193" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L193" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -6664,7 +7826,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J194" t="n">
-        <v>6.397129183475689</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K194" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L194" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -6696,7 +7864,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J195" t="n">
-        <v>5.74756134529847</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K195" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L195" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -6728,7 +7902,13 @@
         <v>1</v>
       </c>
       <c r="J196" t="n">
-        <v>2.465833867631179</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K196" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L196" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -6760,7 +7940,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J197" t="n">
-        <v>2.229883765743884</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K197" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L197" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -6792,7 +7978,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J198" t="n">
-        <v>0.8487044181623319</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K198" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L198" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -6824,7 +8016,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J199" t="n">
-        <v>0.02214262473258277</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K199" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L199" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -6856,7 +8054,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J200" t="n">
-        <v>7.38493506848084</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K200" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L200" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="201">
@@ -6888,7 +8092,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J201" t="n">
-        <v>7.981729011347279</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K201" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L201" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -6920,7 +8130,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J202" t="n">
-        <v>8.074614812005018</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K202" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L202" t="n">
+        <v>7.671768920953231</v>
       </c>
     </row>
     <row r="203">
@@ -6952,7 +8168,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J203" t="n">
-        <v>23.64653493541162</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K203" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L203" t="n">
+        <v>29.07707711526506</v>
       </c>
     </row>
     <row r="204">
@@ -6984,7 +8206,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J204" t="n">
-        <v>29.41353248042616</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K204" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L204" t="n">
+        <v>43.27382382278389</v>
       </c>
     </row>
     <row r="205">
@@ -7016,7 +8244,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J205" t="n">
-        <v>29.54214133544959</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K205" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L205" t="n">
+        <v>41.43592052553375</v>
       </c>
     </row>
     <row r="206">
@@ -7048,7 +8282,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J206" t="n">
-        <v>31.50458075037544</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K206" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L206" t="n">
+        <v>40.51025088011565</v>
       </c>
     </row>
     <row r="207">
@@ -7080,7 +8320,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J207" t="n">
-        <v>30.29567848652841</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K207" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L207" t="n">
+        <v>40.53069025954602</v>
       </c>
     </row>
     <row r="208">
@@ -7112,7 +8358,13 @@
         <v>-1</v>
       </c>
       <c r="J208" t="n">
-        <v>30.84572431098714</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K208" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L208" t="n">
+        <v>40.14565660031623</v>
       </c>
     </row>
     <row r="209">
@@ -7144,7 +8396,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J209" t="n">
-        <v>31.36035953466624</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K209" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L209" t="n">
+        <v>43.42916787436408</v>
       </c>
     </row>
     <row r="210">
@@ -7176,7 +8434,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J210" t="n">
-        <v>31.09355160714052</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K210" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L210" t="n">
+        <v>43.90525097071937</v>
       </c>
     </row>
     <row r="211">
@@ -7208,7 +8472,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J211" t="n">
-        <v>32.40137886557444</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K211" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L211" t="n">
+        <v>41.83225171013407</v>
       </c>
     </row>
     <row r="212">
@@ -7240,7 +8510,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J212" t="n">
-        <v>25.54727492388686</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K212" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L212" t="n">
+        <v>15.8121201809923</v>
       </c>
     </row>
     <row r="213">
@@ -7272,7 +8548,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J213" t="n">
-        <v>9.115601093168319</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K213" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L213" t="n">
+        <v>0.6913041683413574</v>
       </c>
     </row>
     <row r="214">
@@ -7304,7 +8586,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J214" t="n">
-        <v>7.914043474892862</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K214" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L214" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -7336,7 +8624,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J215" t="n">
-        <v>6.549360307076551</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K215" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L215" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="216">
@@ -7368,7 +8662,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J216" t="n">
-        <v>6.973564549734427</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K216" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L216" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -7400,7 +8700,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J217" t="n">
-        <v>2.606293502679467</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K217" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L217" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -7432,7 +8738,13 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="J218" t="n">
-        <v>2.530994190690369</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K218" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L218" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -7464,7 +8776,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J219" t="n">
-        <v>2.259845413619828</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K219" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L219" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="220">
@@ -7496,7 +8814,13 @@
         <v>1</v>
       </c>
       <c r="J220" t="n">
-        <v>1.668582461967508</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K220" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L220" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -7528,7 +8852,13 @@
         <v>0.9659258262890683</v>
       </c>
       <c r="J221" t="n">
-        <v>1.283124161041693</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K221" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L221" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -7560,7 +8890,13 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="J222" t="n">
-        <v>0.9910794589295536</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K222" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L222" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -7592,7 +8928,13 @@
         <v>0.7071067811865476</v>
       </c>
       <c r="J223" t="n">
-        <v>0.1218864700816773</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K223" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L223" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -7624,7 +8966,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J224" t="n">
-        <v>7.260157547654828</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K224" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L224" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="225">
@@ -7656,7 +9004,13 @@
         <v>0.2588190451025207</v>
       </c>
       <c r="J225" t="n">
-        <v>9.249454032492347</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K225" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L225" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -7688,7 +9042,13 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="J226" t="n">
-        <v>7.687565651202401</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K226" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L226" t="n">
+        <v>7.400687193342297</v>
       </c>
     </row>
     <row r="227">
@@ -7720,7 +9080,13 @@
         <v>-0.2588190451025209</v>
       </c>
       <c r="J227" t="n">
-        <v>26.44871712235351</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K227" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L227" t="n">
+        <v>29.20322432942983</v>
       </c>
     </row>
     <row r="228">
@@ -7752,7 +9118,13 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="J228" t="n">
-        <v>33.01533842702588</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K228" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L228" t="n">
+        <v>40.02823586363903</v>
       </c>
     </row>
     <row r="229">
@@ -7784,7 +9156,13 @@
         <v>-0.7071067811865475</v>
       </c>
       <c r="J229" t="n">
-        <v>36.81958553240867</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K229" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L229" t="n">
+        <v>40.58787217541013</v>
       </c>
     </row>
     <row r="230">
@@ -7816,7 +9194,13 @@
         <v>-0.8660254037844387</v>
       </c>
       <c r="J230" t="n">
-        <v>36.90594757993249</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K230" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L230" t="n">
+        <v>41.92305183216878</v>
       </c>
     </row>
     <row r="231">
@@ -7848,7 +9232,13 @@
         <v>-0.9659258262890682</v>
       </c>
       <c r="J231" t="n">
-        <v>36.54216181591646</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K231" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L231" t="n">
+        <v>43.11358602276708</v>
       </c>
     </row>
     <row r="232">
@@ -7880,7 +9270,13 @@
         <v>-1</v>
       </c>
       <c r="J232" t="n">
-        <v>37.32937607460111</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K232" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L232" t="n">
+        <v>44.35064863168498</v>
       </c>
     </row>
     <row r="233">
@@ -7912,7 +9308,13 @@
         <v>-0.9659258262890684</v>
       </c>
       <c r="J233" t="n">
-        <v>28.49226388393222</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K233" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L233" t="n">
+        <v>46.35230127614673</v>
       </c>
     </row>
     <row r="234">
@@ -7944,7 +9346,13 @@
         <v>-0.8660254037844386</v>
       </c>
       <c r="J234" t="n">
-        <v>28.62834635412036</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K234" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L234" t="n">
+        <v>46.37252629606716</v>
       </c>
     </row>
     <row r="235">
@@ -7976,7 +9384,13 @@
         <v>-0.7071067811865477</v>
       </c>
       <c r="J235" t="n">
-        <v>29.33302499021924</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K235" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L235" t="n">
+        <v>44.64943901369155</v>
       </c>
     </row>
     <row r="236">
@@ -8008,7 +9422,13 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="J236" t="n">
-        <v>26.02168973119664</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K236" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L236" t="n">
+        <v>17.66574355125138</v>
       </c>
     </row>
     <row r="237">
@@ -8040,7 +9460,13 @@
         <v>-0.2588190451025206</v>
       </c>
       <c r="J237" t="n">
-        <v>12.23837614895604</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K237" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L237" t="n">
+        <v>0.7212560839840041</v>
       </c>
     </row>
     <row r="238">
@@ -8072,7 +9498,13 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="J238" t="n">
-        <v>7.700293269590694</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K238" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L238" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="239">
@@ -8104,7 +9536,13 @@
         <v>0.2588190451025203</v>
       </c>
       <c r="J239" t="n">
-        <v>7.283542118443312</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K239" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L239" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -8136,7 +9574,13 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="J240" t="n">
-        <v>8.436624725004442</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K240" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L240" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -8168,7 +9612,13 @@
         <v>0.7071067811865474</v>
       </c>
       <c r="J241" t="n">
-        <v>0.5731499887779635</v>
+        <v>1.224646799147353e-16</v>
+      </c>
+      <c r="K241" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L241" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>